<commit_message>
PCA corrected + SFS start
</commit_message>
<xml_diff>
--- a/results/automatic_study_features_rndxCNN.xlsx
+++ b/results/automatic_study_features_rndxCNN.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtros\CS\cours\Cours_de_2A\electifML\geoproject\results\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3A7563-E1D5-4D6B-AEE7-F858B99114A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t>train_f1_score</t>
   </si>
@@ -212,13 +206,61 @@
   </si>
   <si>
     <t>model_dense_6_output_5 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_0 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_1 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_2 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_3 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_4 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_5 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_6 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_7 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_8 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_9 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_10 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_32_output_11 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_16_output_0 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_16_output_1 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_16_output_2 importance</t>
+  </si>
+  <si>
+    <t>PCA_model_dense_16_output_3 importance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,14 +323,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -335,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,27 +401,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -419,24 +435,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -612,16 +610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BL7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CB8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:80">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,398 +810,446 @@
       <c r="BL1" s="1" t="s">
         <v>63</v>
       </c>
+      <c r="BM1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="BO1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="BP1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="BR1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="BV1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="BW1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="BX1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="BY1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB1" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:80">
       <c r="A2">
-        <v>0.99998026921865835</v>
+        <v>0.9999802692186583</v>
       </c>
       <c r="B2">
         <v>20</v>
       </c>
       <c r="C2">
-        <v>0.49852984016975221</v>
+        <v>0.4985298401697522</v>
       </c>
       <c r="D2">
-        <v>2.3786151440083961E-2</v>
+        <v>0.02378615144008396</v>
       </c>
       <c r="E2">
         <v>0.5360343097024155</v>
       </c>
       <c r="F2">
-        <v>0.44372816760476369</v>
+        <v>0.4437281676047637</v>
       </c>
       <c r="G2">
-        <v>4.2073435759932332E-2</v>
+        <v>0.04207343575993233</v>
       </c>
       <c r="H2">
-        <v>2.4450767546992779E-3</v>
+        <v>0.002445076754699278</v>
       </c>
       <c r="I2">
-        <v>2.9288291367903879E-2</v>
+        <v>0.02928829136790388</v>
       </c>
       <c r="J2">
-        <v>9.1249156494976127E-3</v>
+        <v>0.009124915649497613</v>
       </c>
       <c r="K2">
-        <v>4.1591638654742052E-2</v>
+        <v>0.04159163865474205</v>
       </c>
       <c r="L2">
-        <v>2.4025783407189669E-2</v>
+        <v>0.02402578340718967</v>
       </c>
       <c r="M2">
-        <v>2.7292793286012269E-2</v>
+        <v>0.02729279328601227</v>
       </c>
       <c r="N2">
-        <v>5.2152788854156499E-3</v>
+        <v>0.00521527888541565</v>
       </c>
       <c r="O2">
-        <v>6.6360316669138962E-3</v>
+        <v>0.006636031666913896</v>
       </c>
       <c r="P2">
-        <v>1.445986737137094E-3</v>
+        <v>0.001445986737137094</v>
       </c>
       <c r="Q2">
-        <v>4.8028403572834222E-2</v>
+        <v>0.04802840357283422</v>
       </c>
       <c r="R2">
-        <v>2.6189207674028561E-2</v>
+        <v>0.02618920767402856</v>
       </c>
       <c r="S2">
-        <v>2.9495294847972049E-2</v>
+        <v>0.02949529484797205</v>
       </c>
       <c r="T2">
-        <v>2.444104832608926E-2</v>
+        <v>0.02444104832608926</v>
       </c>
       <c r="U2">
-        <v>1.1321854194737319E-2</v>
+        <v>0.01132185419473732</v>
       </c>
       <c r="V2">
-        <v>1.795856753726126E-3</v>
+        <v>0.001795856753726126</v>
       </c>
       <c r="W2">
-        <v>2.1407527636533221E-3</v>
+        <v>0.002140752763653322</v>
       </c>
       <c r="X2">
-        <v>1.1308035949973309E-2</v>
+        <v>0.01130803594997331</v>
       </c>
       <c r="Y2">
-        <v>2.1502273333146089E-2</v>
+        <v>0.02150227333314609</v>
       </c>
       <c r="Z2">
-        <v>5.1697274125774927E-2</v>
+        <v>0.05169727412577493</v>
       </c>
       <c r="AA2">
-        <v>2.4850598022324501E-2</v>
+        <v>0.0248505980223245</v>
       </c>
       <c r="AB2">
-        <v>2.220692769643396E-2</v>
+        <v>0.02220692769643396</v>
       </c>
       <c r="AC2">
-        <v>2.455975336270522E-2</v>
+        <v>0.02455975336270522</v>
       </c>
       <c r="AD2">
-        <v>6.5540191589646121E-2</v>
+        <v>0.06554019158964612</v>
       </c>
       <c r="AE2">
-        <v>7.6436117656629851E-3</v>
+        <v>0.007643611765662985</v>
       </c>
       <c r="AF2">
-        <v>3.5471356227400499E-3</v>
+        <v>0.00354713562274005</v>
       </c>
       <c r="AG2">
-        <v>1.203103441154895E-3</v>
+        <v>0.001203103441154895</v>
       </c>
       <c r="AH2">
-        <v>1.852776358747799E-3</v>
+        <v>0.001852776358747799</v>
       </c>
       <c r="AI2">
-        <v>2.553431664502343E-3</v>
+        <v>0.002553431664502343</v>
       </c>
       <c r="AJ2">
-        <v>2.14248764115006E-2</v>
+        <v>0.0214248764115006</v>
       </c>
       <c r="AK2">
-        <v>5.4263240654830406E-3</v>
+        <v>0.005426324065483041</v>
       </c>
       <c r="AL2">
-        <v>2.481319145075565E-2</v>
+        <v>0.02481319145075565</v>
       </c>
       <c r="AM2">
-        <v>2.2449285374851872E-3</v>
+        <v>0.002244928537485187</v>
       </c>
       <c r="AN2">
-        <v>2.6780314469270969E-3</v>
+        <v>0.002678031446927097</v>
       </c>
       <c r="AO2">
-        <v>3.861091545398192E-3</v>
+        <v>0.003861091545398192</v>
       </c>
       <c r="AP2">
-        <v>6.6957439316160513E-3</v>
+        <v>0.006695743931616051</v>
       </c>
       <c r="AQ2">
-        <v>3.6633207441570452E-5</v>
+        <v>3.663320744157045E-05</v>
       </c>
       <c r="AR2">
-        <v>3.5483452958725223E-2</v>
+        <v>0.03548345295872522</v>
       </c>
       <c r="AS2">
-        <v>6.7075247766895627E-5</v>
+        <v>6.707524776689563E-05</v>
       </c>
       <c r="AT2">
-        <v>2.4945997752576331E-6</v>
+        <v>2.494599775257633E-06</v>
       </c>
       <c r="AU2">
-        <v>4.5116342500521323E-2</v>
+        <v>0.04511634250052132</v>
       </c>
       <c r="AV2">
-        <v>4.2771763893547871E-5</v>
+        <v>4.277176389354787E-05</v>
       </c>
       <c r="AW2">
-        <v>3.7752646535707722E-2</v>
+        <v>0.03775264653570772</v>
       </c>
       <c r="AX2">
-        <v>1.2886723622612219E-3</v>
+        <v>0.001288672362261222</v>
       </c>
       <c r="AY2">
-        <v>7.0452976646410398E-2</v>
+        <v>0.0704529766464104</v>
       </c>
       <c r="AZ2">
-        <v>6.7228410133947239E-3</v>
+        <v>0.006722841013394724</v>
       </c>
       <c r="BA2">
-        <v>5.7116593599471531E-5</v>
+        <v>5.711659359947153E-05</v>
       </c>
       <c r="BB2">
-        <v>3.3649299088524452E-2</v>
+        <v>0.03364929908852445</v>
       </c>
       <c r="BC2">
-        <v>2.332793811340993E-6</v>
+        <v>2.332793811340993E-06</v>
       </c>
       <c r="BD2">
-        <v>8.9080583060589195E-3</v>
+        <v>0.008908058306058919</v>
       </c>
       <c r="BE2">
-        <v>1.796202045462937E-3</v>
+        <v>0.001796202045462937</v>
       </c>
       <c r="BF2">
-        <v>3.5572445940957681E-2</v>
+        <v>0.03557244594095768</v>
       </c>
       <c r="BG2">
-        <v>4.1175036433703688E-5</v>
+        <v>4.117503643370369E-05</v>
       </c>
       <c r="BH2">
-        <v>3.2439713898945302E-2</v>
+        <v>0.0324397138989453</v>
       </c>
       <c r="BI2">
-        <v>6.78360944776739E-5</v>
+        <v>6.78360944776739E-05</v>
       </c>
       <c r="BJ2">
-        <v>3.042273159688854E-6</v>
+        <v>3.042273159688854E-06</v>
       </c>
       <c r="BK2">
-        <v>5.2293395506657389E-2</v>
+        <v>0.05229339550665739</v>
       </c>
       <c r="BL2">
-        <v>4.2524961550905713E-5</v>
+        <v>4.252496155090571E-05</v>
       </c>
     </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:80">
       <c r="A3">
-        <v>0.99999401138750887</v>
+        <v>0.9999940113875089</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>0.50830824546870312</v>
+        <v>0.5083082454687031</v>
       </c>
       <c r="D3">
-        <v>1.838159773448873E-2</v>
+        <v>0.01838159773448873</v>
       </c>
       <c r="E3">
-        <v>0.53912041758724605</v>
+        <v>0.539120417587246</v>
       </c>
       <c r="F3">
-        <v>0.48191303669913987</v>
+        <v>0.4819130366991399</v>
       </c>
       <c r="G3">
-        <v>4.3099720562001689E-2</v>
+        <v>0.04309972056200169</v>
       </c>
       <c r="H3">
-        <v>2.3976485324070521E-3</v>
+        <v>0.002397648532407052</v>
       </c>
       <c r="I3">
-        <v>2.9332595820356119E-2</v>
+        <v>0.02933259582035612</v>
       </c>
       <c r="J3">
-        <v>9.074412520270695E-3</v>
+        <v>0.009074412520270695</v>
       </c>
       <c r="K3">
-        <v>4.5107919216988791E-2</v>
+        <v>0.04510791921698879</v>
       </c>
       <c r="L3">
-        <v>2.292478221415107E-2</v>
+        <v>0.02292478221415107</v>
       </c>
       <c r="M3">
-        <v>2.4475896158433871E-2</v>
+        <v>0.02447589615843387</v>
       </c>
       <c r="N3">
-        <v>5.2161214862173197E-3</v>
+        <v>0.00521612148621732</v>
       </c>
       <c r="O3">
-        <v>7.2070100411722789E-3</v>
+        <v>0.007207010041172279</v>
       </c>
       <c r="P3">
-        <v>1.652517023658962E-3</v>
+        <v>0.001652517023658962</v>
       </c>
       <c r="Q3">
-        <v>4.9473098485783337E-2</v>
+        <v>0.04947309848578334</v>
       </c>
       <c r="R3">
-        <v>2.6740454548114641E-2</v>
+        <v>0.02674045454811464</v>
       </c>
       <c r="S3">
-        <v>2.6321108779155E-2</v>
+        <v>0.026321108779155</v>
       </c>
       <c r="T3">
-        <v>2.3259740414906312E-2</v>
+        <v>0.02325974041490631</v>
       </c>
       <c r="U3">
-        <v>1.1750287670476801E-2</v>
+        <v>0.0117502876704768</v>
       </c>
       <c r="V3">
-        <v>1.855380830570289E-3</v>
+        <v>0.001855380830570289</v>
       </c>
       <c r="W3">
-        <v>2.147249152855738E-3</v>
+        <v>0.002147249152855738</v>
       </c>
       <c r="X3">
-        <v>1.116894305752013E-2</v>
+        <v>0.01116894305752013</v>
       </c>
       <c r="Y3">
-        <v>2.13497207597887E-2</v>
+        <v>0.0213497207597887</v>
       </c>
       <c r="Z3">
-        <v>5.2546915511057647E-2</v>
+        <v>0.05254691551105765</v>
       </c>
       <c r="AA3">
-        <v>2.5602585513269091E-2</v>
+        <v>0.02560258551326909</v>
       </c>
       <c r="AB3">
-        <v>2.1364881546480651E-2</v>
+        <v>0.02136488154648065</v>
       </c>
       <c r="AC3">
-        <v>2.4373239983630109E-2</v>
+        <v>0.02437323998363011</v>
       </c>
       <c r="AD3">
-        <v>6.3846231628347155E-2</v>
+        <v>0.06384623162834716</v>
       </c>
       <c r="AE3">
-        <v>7.7203279416660298E-3</v>
+        <v>0.00772032794166603</v>
       </c>
       <c r="AF3">
-        <v>3.1919626291825789E-3</v>
+        <v>0.003191962629182579</v>
       </c>
       <c r="AG3">
-        <v>1.2138649332481099E-3</v>
+        <v>0.00121386493324811</v>
       </c>
       <c r="AH3">
-        <v>1.8117801590237571E-3</v>
+        <v>0.001811780159023757</v>
       </c>
       <c r="AI3">
-        <v>2.5808078714800202E-3</v>
+        <v>0.00258080787148002</v>
       </c>
       <c r="AJ3">
-        <v>2.3522961771920241E-2</v>
+        <v>0.02352296177192024</v>
       </c>
       <c r="AK3">
-        <v>5.8723657940842567E-3</v>
+        <v>0.005872365794084257</v>
       </c>
       <c r="AL3">
-        <v>2.6448764732355651E-2</v>
+        <v>0.02644876473235565</v>
       </c>
       <c r="AM3">
-        <v>2.272922677013151E-3</v>
+        <v>0.002272922677013151</v>
       </c>
       <c r="AN3">
-        <v>2.6890529762950868E-3</v>
+        <v>0.002689052976295087</v>
       </c>
       <c r="AO3">
-        <v>3.7707008926102059E-3</v>
+        <v>0.003770700892610206</v>
       </c>
       <c r="AP3">
-        <v>6.5189481480701248E-3</v>
+        <v>0.006518948148070125</v>
       </c>
       <c r="AQ3">
-        <v>3.8123510069889348E-5</v>
+        <v>3.812351006988935E-05</v>
       </c>
       <c r="AR3">
-        <v>3.6518753848032028E-2</v>
+        <v>0.03651875384803203</v>
       </c>
       <c r="AS3">
-        <v>7.8394647209753491E-5</v>
+        <v>7.839464720975349E-05</v>
       </c>
       <c r="AT3">
-        <v>3.4513141033246189E-6</v>
+        <v>3.451314103324619E-06</v>
       </c>
       <c r="AU3">
-        <v>4.8116828999039442E-2</v>
+        <v>0.04811682899903944</v>
       </c>
       <c r="AV3">
-        <v>4.569988684457845E-5</v>
+        <v>4.569988684457845E-05</v>
       </c>
       <c r="AW3">
-        <v>2.9254969328927641E-2</v>
+        <v>0.02925496932892764</v>
       </c>
       <c r="AX3">
-        <v>1.2627667543931361E-3</v>
+        <v>0.001262766754393136</v>
       </c>
       <c r="AY3">
-        <v>7.2466074108283207E-2</v>
+        <v>0.07246607410828321</v>
       </c>
       <c r="AZ3">
-        <v>6.957482089709509E-3</v>
+        <v>0.006957482089709509</v>
       </c>
       <c r="BA3">
-        <v>6.0453065590241638E-5</v>
+        <v>6.045306559024164E-05</v>
       </c>
       <c r="BB3">
-        <v>3.4946808898102033E-2</v>
+        <v>0.03494680889810203</v>
       </c>
       <c r="BC3">
-        <v>2.1756981271878142E-6</v>
+        <v>2.175698127187814E-06</v>
       </c>
       <c r="BD3">
-        <v>8.6569833954176518E-3</v>
+        <v>0.008656983395417652</v>
       </c>
       <c r="BE3">
-        <v>1.242061937927917E-3</v>
+        <v>0.001242061937927917</v>
       </c>
       <c r="BF3">
-        <v>3.6253233688826672E-2</v>
+        <v>0.03625323368882667</v>
       </c>
       <c r="BG3">
-        <v>3.5915655478993943E-5</v>
+        <v>3.591565547899394E-05</v>
       </c>
       <c r="BH3">
-        <v>3.2554336718762462E-2</v>
+        <v>0.03255433671876246</v>
       </c>
       <c r="BI3">
-        <v>7.3713322381183154E-5</v>
+        <v>7.371332238118315E-05</v>
       </c>
       <c r="BJ3">
-        <v>4.0926487460882651E-6</v>
+        <v>4.092648746088265E-06</v>
       </c>
       <c r="BK3">
-        <v>5.1479412885224451E-2</v>
+        <v>0.05147941288522445</v>
       </c>
       <c r="BL3">
-        <v>4.5345614240006359E-5</v>
+        <v>4.534561424000636E-05</v>
       </c>
     </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:80">
       <c r="A4">
-        <v>0.99992676782111267</v>
+        <v>0.9999267678211127</v>
       </c>
       <c r="B4">
         <v>5</v>
@@ -1214,25 +1258,25 @@
         <v>0.4618164238799527</v>
       </c>
       <c r="D4">
-        <v>1.9834376078437611E-2</v>
+        <v>0.01983437607843761</v>
       </c>
       <c r="E4">
-        <v>0.49208004728832783</v>
+        <v>0.4920800472883278</v>
       </c>
       <c r="F4">
-        <v>0.43078935968124799</v>
+        <v>0.430789359681248</v>
       </c>
       <c r="G4">
-        <v>0.13078049679947279</v>
+        <v>0.1307804967994728</v>
       </c>
       <c r="H4">
-        <v>6.8773640277492477E-3</v>
+        <v>0.006877364027749248</v>
       </c>
       <c r="I4">
         <v>0.1107234059327494</v>
       </c>
       <c r="J4">
-        <v>3.3160252094670911E-2</v>
+        <v>0.03316025209467091</v>
       </c>
       <c r="K4">
         <v>0.1726475466045414</v>
@@ -1244,355 +1288,435 @@
         <v>0.1804958569066662</v>
       </c>
       <c r="AD4">
-        <v>0.18482130105027161</v>
+        <v>0.1848213010502716</v>
       </c>
     </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:80">
       <c r="A5">
-        <v>0.99991757314577445</v>
+        <v>0.9999175731457745</v>
       </c>
       <c r="B5">
         <v>20</v>
       </c>
       <c r="C5">
-        <v>0.45563207413148582</v>
+        <v>0.4556320741314858</v>
       </c>
       <c r="D5">
-        <v>2.37414047805782E-2</v>
+        <v>0.0237414047805782</v>
       </c>
       <c r="E5">
-        <v>0.50544567025190668</v>
+        <v>0.5054456702519067</v>
       </c>
       <c r="F5">
-        <v>0.40375826479322879</v>
+        <v>0.4037582647932288</v>
       </c>
       <c r="G5">
-        <v>0.13295973203118799</v>
+        <v>0.132959732031188</v>
       </c>
       <c r="H5">
-        <v>6.760517620738476E-3</v>
+        <v>0.006760517620738476</v>
       </c>
       <c r="I5">
-        <v>0.11053582992774651</v>
+        <v>0.1105358299277465</v>
       </c>
       <c r="J5">
-        <v>3.3076582727133513E-2</v>
+        <v>0.03307658272713351</v>
       </c>
       <c r="K5">
-        <v>0.16015068895706569</v>
+        <v>0.1601506889570657</v>
       </c>
       <c r="Q5">
-        <v>0.19214030310814381</v>
+        <v>0.1921403031081438</v>
       </c>
       <c r="Z5">
-        <v>0.17810241504269181</v>
+        <v>0.1781024150426918</v>
       </c>
       <c r="AD5">
-        <v>0.18627393058529221</v>
+        <v>0.1862739305852922</v>
       </c>
     </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:80">
       <c r="A6">
-        <v>0.99993090924254202</v>
+        <v>0.999930909242542</v>
       </c>
       <c r="B6">
         <v>40</v>
       </c>
       <c r="C6">
-        <v>0.50259225932370155</v>
+        <v>0.5025922593237016</v>
       </c>
       <c r="D6">
-        <v>3.5099590945420422E-2</v>
+        <v>0.03509959094542042</v>
       </c>
       <c r="E6">
-        <v>0.56668181430707143</v>
+        <v>0.5666818143070714</v>
       </c>
       <c r="F6">
-        <v>0.43924862629096267</v>
+        <v>0.4392486262909627</v>
       </c>
       <c r="G6">
-        <v>6.3755545806494993E-2</v>
+        <v>0.06375554580649499</v>
       </c>
       <c r="H6">
-        <v>3.904688311976651E-3</v>
+        <v>0.003904688311976651</v>
       </c>
       <c r="I6">
-        <v>4.9013651511526403E-2</v>
+        <v>0.0490136515115264</v>
       </c>
       <c r="J6">
-        <v>1.6982945249987998E-2</v>
+        <v>0.016982945249988</v>
       </c>
       <c r="K6">
-        <v>6.5041108026980141E-2</v>
+        <v>0.06504110802698014</v>
       </c>
       <c r="Q6">
-        <v>7.1645141926158826E-2</v>
+        <v>0.07164514192615883</v>
       </c>
       <c r="Z6">
-        <v>8.1111783145610322E-2</v>
+        <v>0.08111178314561032</v>
       </c>
       <c r="AD6">
-        <v>8.5174554829123617E-2</v>
+        <v>0.08517455482912362</v>
       </c>
       <c r="AQ6">
-        <v>8.8486880279090593E-5</v>
+        <v>8.848688027909059E-05</v>
       </c>
       <c r="AR6">
-        <v>5.6994050830427072E-2</v>
+        <v>0.05699405083042707</v>
       </c>
       <c r="AS6">
-        <v>1.3906917884454309E-4</v>
+        <v>0.0001390691788445431</v>
       </c>
       <c r="AT6">
-        <v>8.9243609918509879E-6</v>
+        <v>8.924360991850988E-06</v>
       </c>
       <c r="AU6">
-        <v>7.7366423953632704E-2</v>
+        <v>0.0773664239536327</v>
       </c>
       <c r="AV6">
-        <v>9.4652110456306388E-5</v>
+        <v>9.465211045630639E-05</v>
       </c>
       <c r="AW6">
-        <v>4.398130679978348E-2</v>
+        <v>0.04398130679978348</v>
       </c>
       <c r="AX6">
-        <v>2.4551409651989622E-3</v>
+        <v>0.002455140965198962</v>
       </c>
       <c r="AY6">
-        <v>9.9332600212671318E-2</v>
+        <v>0.09933260021267132</v>
       </c>
       <c r="AZ6">
-        <v>1.381017723250883E-2</v>
+        <v>0.01381017723250883</v>
       </c>
       <c r="BA6">
-        <v>1.2230325385126351E-4</v>
+        <v>0.0001223032538512635</v>
       </c>
       <c r="BB6">
-        <v>5.9444386436893683E-2</v>
+        <v>0.05944438643689368</v>
       </c>
       <c r="BC6">
-        <v>3.042160990292472E-6</v>
+        <v>3.042160990292472E-06</v>
       </c>
       <c r="BD6">
-        <v>1.6000123115793189E-2</v>
+        <v>0.01600012311579319</v>
       </c>
       <c r="BE6">
-        <v>2.8279331915245752E-3</v>
+        <v>0.002827933191524575</v>
       </c>
       <c r="BF6">
-        <v>6.3074047609119402E-2</v>
+        <v>0.0630740476091194</v>
       </c>
       <c r="BG6">
-        <v>8.6739077891691223E-5</v>
+        <v>8.673907789169122E-05</v>
       </c>
       <c r="BH6">
-        <v>5.3028270567429793E-2</v>
+        <v>0.05302827056742979</v>
       </c>
       <c r="BI6">
-        <v>1.2854599592694319E-4</v>
+        <v>0.0001285459959269432</v>
       </c>
       <c r="BJ6">
-        <v>6.0584351453147441E-6</v>
+        <v>6.058435145314744E-06</v>
       </c>
       <c r="BK6">
-        <v>7.4279906636428986E-2</v>
+        <v>0.07427990663642899</v>
       </c>
       <c r="BL6">
-        <v>9.8392186351895655E-5</v>
+        <v>9.839218635189565E-05</v>
       </c>
     </row>
-    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:80">
       <c r="A7">
-        <v>0.99993230049437198</v>
+        <v>0.999932300494372</v>
       </c>
       <c r="B7">
         <v>40</v>
       </c>
       <c r="C7">
-        <v>0.49619831376572998</v>
+        <v>0.49619831376573</v>
       </c>
       <c r="D7">
-        <v>3.6343407908627931E-2</v>
+        <v>0.03634340790862793</v>
       </c>
       <c r="E7">
-        <v>0.57198231489993723</v>
+        <v>0.5719823148999372</v>
       </c>
       <c r="F7">
         <v>0.4232037973257074</v>
       </c>
       <c r="G7">
-        <v>4.2164787113776837E-2</v>
+        <v>0.04216478711377684</v>
       </c>
       <c r="H7">
-        <v>2.414124001275737E-3</v>
+        <v>0.002414124001275737</v>
       </c>
       <c r="I7">
-        <v>2.8949803787809252E-2</v>
+        <v>0.02894980378780925</v>
       </c>
       <c r="J7">
-        <v>9.0239700152618986E-3</v>
+        <v>0.009023970015261899</v>
       </c>
       <c r="K7">
-        <v>4.4595962978386181E-2</v>
+        <v>0.04459596297838618</v>
       </c>
       <c r="L7">
-        <v>2.2762698669471872E-2</v>
+        <v>0.02276269866947187</v>
       </c>
       <c r="M7">
-        <v>3.1110426832507521E-2</v>
+        <v>0.03111042683250752</v>
       </c>
       <c r="N7">
-        <v>5.1574459659131716E-3</v>
+        <v>0.005157445965913172</v>
       </c>
       <c r="O7">
-        <v>6.6740947280266132E-3</v>
+        <v>0.006674094728026613</v>
       </c>
       <c r="P7">
-        <v>1.5941566276171061E-3</v>
+        <v>0.001594156627617106</v>
       </c>
       <c r="Q7">
-        <v>4.76318358793692E-2</v>
+        <v>0.0476318358793692</v>
       </c>
       <c r="R7">
-        <v>2.53834260608953E-2</v>
+        <v>0.0253834260608953</v>
       </c>
       <c r="S7">
-        <v>2.4456280860145091E-2</v>
+        <v>0.02445628086014509</v>
       </c>
       <c r="T7">
-        <v>2.2922644239387651E-2</v>
+        <v>0.02292264423938765</v>
       </c>
       <c r="U7">
-        <v>1.147918943258429E-2</v>
+        <v>0.01147918943258429</v>
       </c>
       <c r="V7">
-        <v>1.801127445663252E-3</v>
+        <v>0.001801127445663252</v>
       </c>
       <c r="W7">
-        <v>2.15209489729767E-3</v>
+        <v>0.00215209489729767</v>
       </c>
       <c r="X7">
-        <v>1.1453324971996019E-2</v>
+        <v>0.01145332497199602</v>
       </c>
       <c r="Y7">
-        <v>2.1634180693684699E-2</v>
+        <v>0.0216341806936847</v>
       </c>
       <c r="Z7">
-        <v>5.8344355078838811E-2</v>
+        <v>0.05834435507883881</v>
       </c>
       <c r="AA7">
-        <v>2.6015870940667821E-2</v>
+        <v>0.02601587094066782</v>
       </c>
       <c r="AB7">
-        <v>2.1567226806941439E-2</v>
+        <v>0.02156722680694144</v>
       </c>
       <c r="AC7">
-        <v>2.4437616626742469E-2</v>
+        <v>0.02443761662674247</v>
       </c>
       <c r="AD7">
-        <v>6.4672663137336148E-2</v>
+        <v>0.06467266313733615</v>
       </c>
       <c r="AE7">
-        <v>7.4858258598917062E-3</v>
+        <v>0.007485825859891706</v>
       </c>
       <c r="AF7">
-        <v>3.0577317015329912E-3</v>
+        <v>0.003057731701532991</v>
       </c>
       <c r="AG7">
-        <v>1.1878764682757531E-3</v>
+        <v>0.001187876468275753</v>
       </c>
       <c r="AH7">
-        <v>1.909155128761376E-3</v>
+        <v>0.001909155128761376</v>
       </c>
       <c r="AI7">
-        <v>2.545897662478236E-3</v>
+        <v>0.002545897662478236</v>
       </c>
       <c r="AJ7">
-        <v>2.2492369471632152E-2</v>
+        <v>0.02249236947163215</v>
       </c>
       <c r="AK7">
-        <v>6.2150420407168392E-3</v>
+        <v>0.006215042040716839</v>
       </c>
       <c r="AL7">
-        <v>2.578603798049996E-2</v>
+        <v>0.02578603798049996</v>
       </c>
       <c r="AM7">
-        <v>2.2751661241403199E-3</v>
+        <v>0.00227516612414032</v>
       </c>
       <c r="AN7">
-        <v>2.7200791137789201E-3</v>
+        <v>0.00272007911377892</v>
       </c>
       <c r="AO7">
-        <v>3.8270451215220492E-3</v>
+        <v>0.003827045121522049</v>
       </c>
       <c r="AP7">
-        <v>6.5705996965496408E-3</v>
+        <v>0.006570599696549641</v>
       </c>
       <c r="AQ7">
-        <v>3.5643074314555822E-5</v>
+        <v>3.564307431455582E-05</v>
       </c>
       <c r="AR7">
-        <v>3.4581391719577401E-2</v>
+        <v>0.0345813917195774</v>
       </c>
       <c r="AS7">
-        <v>7.4778302595773506E-5</v>
+        <v>7.477830259577351E-05</v>
       </c>
       <c r="AT7">
-        <v>2.3329780729643868E-6</v>
+        <v>2.332978072964387E-06</v>
       </c>
       <c r="AU7">
-        <v>5.4199276627574289E-2</v>
+        <v>0.05419927662757429</v>
       </c>
       <c r="AV7">
-        <v>4.243567815218249E-5</v>
+        <v>4.243567815218249E-05</v>
       </c>
       <c r="AW7">
-        <v>2.9074396697862728E-2</v>
+        <v>0.02907439669786273</v>
       </c>
       <c r="AX7">
-        <v>1.321305484345696E-3</v>
+        <v>0.001321305484345696</v>
       </c>
       <c r="AY7">
-        <v>7.2485264592549559E-2</v>
+        <v>0.07248526459254956</v>
       </c>
       <c r="AZ7">
-        <v>7.2822162875098356E-3</v>
+        <v>0.007282216287509836</v>
       </c>
       <c r="BA7">
-        <v>6.212117192187902E-5</v>
+        <v>6.212117192187902E-05</v>
       </c>
       <c r="BB7">
-        <v>3.6218305928746052E-2</v>
+        <v>0.03621830592874605</v>
       </c>
       <c r="BC7">
-        <v>2.6460701961983182E-6</v>
+        <v>2.646070196198318E-06</v>
       </c>
       <c r="BD7">
-        <v>8.8760080773717699E-3</v>
+        <v>0.00887600807737177</v>
       </c>
       <c r="BE7">
-        <v>2.3337090198141761E-3</v>
+        <v>0.002333709019814176</v>
       </c>
       <c r="BF7">
-        <v>3.601616741790245E-2</v>
+        <v>0.03601616741790245</v>
       </c>
       <c r="BG7">
-        <v>3.8487927353727432E-5</v>
+        <v>3.848792735372743E-05</v>
       </c>
       <c r="BH7">
-        <v>3.4035439649842257E-2</v>
+        <v>0.03403543964984226</v>
       </c>
       <c r="BI7">
-        <v>6.8271737702349874E-5</v>
+        <v>6.827173770234987E-05</v>
       </c>
       <c r="BJ7">
-        <v>2.616743074806342E-6</v>
+        <v>2.616743074806342E-06</v>
       </c>
       <c r="BK7">
-        <v>3.8726917935741033E-2</v>
+        <v>0.03872691793574103</v>
       </c>
       <c r="BL7">
-        <v>4.8132716402358781E-5</v>
+        <v>4.813271640235878E-05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:80">
+      <c r="A8">
+        <v>0.9999972175022197</v>
+      </c>
+      <c r="B8">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>0.5486301773758064</v>
+      </c>
+      <c r="D8">
+        <v>0.01029423128690497</v>
+      </c>
+      <c r="E8">
+        <v>0.5633201781999565</v>
+      </c>
+      <c r="F8">
+        <v>0.5298317981658773</v>
+      </c>
+      <c r="G8">
+        <v>0.06397796689902732</v>
+      </c>
+      <c r="H8">
+        <v>0.002266520493634809</v>
+      </c>
+      <c r="I8">
+        <v>0.03535079426427134</v>
+      </c>
+      <c r="J8">
+        <v>0.01050423920860266</v>
+      </c>
+      <c r="BM8">
+        <v>0.03984066441008055</v>
+      </c>
+      <c r="BN8">
+        <v>0.05516322053075325</v>
+      </c>
+      <c r="BO8">
+        <v>0.07962050867702015</v>
+      </c>
+      <c r="BP8">
+        <v>0.07461725168387211</v>
+      </c>
+      <c r="BQ8">
+        <v>0.06961474993311663</v>
+      </c>
+      <c r="BR8">
+        <v>0.03529056999609417</v>
+      </c>
+      <c r="BS8">
+        <v>0.03076375406550665</v>
+      </c>
+      <c r="BT8">
+        <v>0.04528849524931228</v>
+      </c>
+      <c r="BU8">
+        <v>0.03082261807805221</v>
+      </c>
+      <c r="BV8">
+        <v>0.03490381546225779</v>
+      </c>
+      <c r="BW8">
+        <v>0.04063722471022402</v>
+      </c>
+      <c r="BX8">
+        <v>0.04999402791620833</v>
+      </c>
+      <c r="BY8">
+        <v>0.06750081636007194</v>
+      </c>
+      <c r="BZ8">
+        <v>0.04942823645448381</v>
+      </c>
+      <c r="CA8">
+        <v>0.1131362200519838</v>
+      </c>
+      <c r="CB8">
+        <v>0.07127830555542623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
greedy approach and bye PCA"
</commit_message>
<xml_diff>
--- a/results/automatic_study_features_rndxCNN.xlsx
+++ b/results/automatic_study_features_rndxCNN.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>train_f1_score</t>
   </si>
@@ -254,6 +254,66 @@
   </si>
   <si>
     <t>PCA_model_dense_16_output_3 importance</t>
+  </si>
+  <si>
+    <t>diameters importance</t>
+  </si>
+  <si>
+    <t>ratio_area_over_diameter importance</t>
+  </si>
+  <si>
+    <t>ratio_perimeter_over_diameter importance</t>
+  </si>
+  <si>
+    <t>Dense Urban importance</t>
+  </si>
+  <si>
+    <t>Industrial importance</t>
+  </si>
+  <si>
+    <t>N,A importance</t>
+  </si>
+  <si>
+    <t>Rural importance</t>
+  </si>
+  <si>
+    <t>Sparse Urban importance</t>
+  </si>
+  <si>
+    <t>Urban Slum importance</t>
+  </si>
+  <si>
+    <t>Barren Land importance</t>
+  </si>
+  <si>
+    <t>Coastal importance</t>
+  </si>
+  <si>
+    <t>Dense Forest importance</t>
+  </si>
+  <si>
+    <t>Desert importance</t>
+  </si>
+  <si>
+    <t>Farms importance</t>
+  </si>
+  <si>
+    <t>Grass Land importance</t>
+  </si>
+  <si>
+    <t>Hills importance</t>
+  </si>
+  <si>
+    <t>Lakes importance</t>
+  </si>
+  <si>
+    <t>River importance</t>
+  </si>
+  <si>
+    <t>Snow importance</t>
+  </si>
+  <si>
+    <t>Sparse Forest importance</t>
   </si>
 </sst>
 </file>
@@ -611,13 +671,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:CB8"/>
+  <dimension ref="A1:CV11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:80">
+    <row r="1" spans="1:100">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -858,8 +918,68 @@
       <c r="CB1" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="CC1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="CF1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="CH1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="CK1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="CL1" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="CM1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CN1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="CO1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="CP1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CQ1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="CR1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="CS1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="CT1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="CV1" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="2" spans="1:80">
+    <row r="2" spans="1:100">
       <c r="A2">
         <v>0.9999802692186583</v>
       </c>
@@ -1053,7 +1173,7 @@
         <v>4.252496155090571E-05</v>
       </c>
     </row>
-    <row r="3" spans="1:80">
+    <row r="3" spans="1:100">
       <c r="A3">
         <v>0.9999940113875089</v>
       </c>
@@ -1247,7 +1367,7 @@
         <v>4.534561424000636E-05</v>
       </c>
     </row>
-    <row r="4" spans="1:80">
+    <row r="4" spans="1:100">
       <c r="A4">
         <v>0.9999267678211127</v>
       </c>
@@ -1291,7 +1411,7 @@
         <v>0.1848213010502716</v>
       </c>
     </row>
-    <row r="5" spans="1:80">
+    <row r="5" spans="1:100">
       <c r="A5">
         <v>0.9999175731457745</v>
       </c>
@@ -1335,7 +1455,7 @@
         <v>0.1862739305852922</v>
       </c>
     </row>
-    <row r="6" spans="1:80">
+    <row r="6" spans="1:100">
       <c r="A6">
         <v>0.999930909242542</v>
       </c>
@@ -1445,7 +1565,7 @@
         <v>9.839218635189565E-05</v>
       </c>
     </row>
-    <row r="7" spans="1:80">
+    <row r="7" spans="1:100">
       <c r="A7">
         <v>0.999932300494372</v>
       </c>
@@ -1639,7 +1759,7 @@
         <v>4.813271640235878E-05</v>
       </c>
     </row>
-    <row r="8" spans="1:80">
+    <row r="8" spans="1:100">
       <c r="A8">
         <v>0.9999972175022197</v>
       </c>
@@ -1717,6 +1837,252 @@
       </c>
       <c r="CB8">
         <v>0.07127830555542623</v>
+      </c>
+    </row>
+    <row r="9" spans="1:100">
+      <c r="A9">
+        <v>0.9999944350044395</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>0.5501898162519842</v>
+      </c>
+      <c r="D9">
+        <v>0.01069409847699901</v>
+      </c>
+      <c r="E9">
+        <v>0.5643725361706374</v>
+      </c>
+      <c r="F9">
+        <v>0.5277711643627568</v>
+      </c>
+      <c r="G9">
+        <v>0.04046192694419542</v>
+      </c>
+      <c r="H9">
+        <v>0.001464931012790026</v>
+      </c>
+      <c r="I9">
+        <v>0.02663389284411285</v>
+      </c>
+      <c r="BM9">
+        <v>0.03578403188927403</v>
+      </c>
+      <c r="BN9">
+        <v>0.04770310805630882</v>
+      </c>
+      <c r="BO9">
+        <v>0.06887897750582037</v>
+      </c>
+      <c r="BP9">
+        <v>0.06438403119721645</v>
+      </c>
+      <c r="BQ9">
+        <v>0.06463231681652754</v>
+      </c>
+      <c r="BR9">
+        <v>0.03078707204472345</v>
+      </c>
+      <c r="BS9">
+        <v>0.02704967297420518</v>
+      </c>
+      <c r="BT9">
+        <v>0.04392286493728839</v>
+      </c>
+      <c r="BU9">
+        <v>0.02828644428033223</v>
+      </c>
+      <c r="BV9">
+        <v>0.02998898036313816</v>
+      </c>
+      <c r="BW9">
+        <v>0.035634589507616</v>
+      </c>
+      <c r="BX9">
+        <v>0.05346282437410078</v>
+      </c>
+      <c r="BY9">
+        <v>0.06300635678054092</v>
+      </c>
+      <c r="BZ9">
+        <v>0.04510933351600396</v>
+      </c>
+      <c r="CA9">
+        <v>0.09562962604518779</v>
+      </c>
+      <c r="CB9">
+        <v>0.05559398111673422</v>
+      </c>
+      <c r="CC9">
+        <v>0.04507233458906522</v>
+      </c>
+      <c r="CD9">
+        <v>0.03421069038514324</v>
+      </c>
+      <c r="CE9">
+        <v>0.02718842319100677</v>
+      </c>
+      <c r="CF9">
+        <v>0.003194083152655299</v>
+      </c>
+      <c r="CG9">
+        <v>0.004131048652010479</v>
+      </c>
+      <c r="CH9">
+        <v>0.0008464665507843835</v>
+      </c>
+      <c r="CI9">
+        <v>0.001511044199975395</v>
+      </c>
+      <c r="CJ9">
+        <v>0.002719765276100597</v>
+      </c>
+      <c r="CK9">
+        <v>0.0005964622677658069</v>
+      </c>
+      <c r="CL9">
+        <v>0.002509501656698289</v>
+      </c>
+      <c r="CM9">
+        <v>0.0009051818815880179</v>
+      </c>
+      <c r="CN9">
+        <v>0.002811984509269405</v>
+      </c>
+      <c r="CO9">
+        <v>0.0007595730743912825</v>
+      </c>
+      <c r="CP9">
+        <v>0.002556805851846755</v>
+      </c>
+      <c r="CQ9">
+        <v>0.003016809673591287</v>
+      </c>
+      <c r="CR9">
+        <v>0.0002974563909251212</v>
+      </c>
+      <c r="CS9">
+        <v>0.002442971905166405</v>
+      </c>
+      <c r="CT9">
+        <v>0.002167722924020633</v>
+      </c>
+      <c r="CU9">
+        <v>2.588713083851896E-06</v>
+      </c>
+      <c r="CV9">
+        <v>0.002753789733325153</v>
+      </c>
+    </row>
+    <row r="10" spans="1:100">
+      <c r="A10">
+        <v>0.9999235361075586</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>0.4015086606573693</v>
+      </c>
+      <c r="D10">
+        <v>0.01604397074603381</v>
+      </c>
+      <c r="E10">
+        <v>0.422281829105335</v>
+      </c>
+      <c r="F10">
+        <v>0.3707669628383456</v>
+      </c>
+      <c r="G10">
+        <v>0.1792748421384689</v>
+      </c>
+      <c r="H10">
+        <v>0.006445515156503034</v>
+      </c>
+      <c r="I10">
+        <v>0.143966692240987</v>
+      </c>
+      <c r="J10">
+        <v>0.04729127206912419</v>
+      </c>
+      <c r="K10">
+        <v>0.1361580941790445</v>
+      </c>
+      <c r="Q10">
+        <v>0.1843413663405821</v>
+      </c>
+      <c r="Z10">
+        <v>0.04420786344941158</v>
+      </c>
+      <c r="AD10">
+        <v>0.03709751488524476</v>
+      </c>
+      <c r="AR10">
+        <v>0.1780104094960045</v>
+      </c>
+      <c r="AU10">
+        <v>0.007312474340219226</v>
+      </c>
+      <c r="AY10">
+        <v>0.03415793323395745</v>
+      </c>
+      <c r="AZ10">
+        <v>0.001736022470452692</v>
+      </c>
+    </row>
+    <row r="11" spans="1:100">
+      <c r="A11">
+        <v>0.9999894140928548</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>0.5621231752929592</v>
+      </c>
+      <c r="D11">
+        <v>0.01712064865790634</v>
+      </c>
+      <c r="E11">
+        <v>0.5961625851438895</v>
+      </c>
+      <c r="F11">
+        <v>0.5407715302800719</v>
+      </c>
+      <c r="G11">
+        <v>0.09616565571993174</v>
+      </c>
+      <c r="H11">
+        <v>0.004022001592029104</v>
+      </c>
+      <c r="I11">
+        <v>0.07180985280186022</v>
+      </c>
+      <c r="J11">
+        <v>0.02376138180011252</v>
+      </c>
+      <c r="K11">
+        <v>0.07069688658275719</v>
+      </c>
+      <c r="Q11">
+        <v>0.103487458720009</v>
+      </c>
+      <c r="Z11">
+        <v>0.0216368817431187</v>
+      </c>
+      <c r="AD11">
+        <v>0.02070309470781175</v>
+      </c>
+      <c r="AR11">
+        <v>0.08754080281299732</v>
+      </c>
+      <c r="AW11">
+        <v>0.2231745937029853</v>
+      </c>
+      <c r="BF11">
+        <v>0.2770013898163872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>